<commit_message>
Add extended renovation pricing data and fix matcher compatibility
Added 22 more renovation items to the prijzenboek:
- Container items (afval/puincontainer 3-15 m3): 8 items
- Schoonmaak items (woning reinigen, radiator, sanitair): 13 items
- Updated existing items with correct € notation

Bug fixes:
- Remove btw_laag reference from matcher.py (field no longer exists)
- Add omschrijving_offerte, materiaal, uren, prijs_per_stuk to match results
- Improve unit normalization to support won, woning, ruimte, m3 units

New tools:
- TSV import script for € notation data (€ 6,285.20 format)
- Handles negative values (-€ 249.78)
- Auto-strips thousands separator (6,285.20 -> 6285.20)

The prijzenboek now contains 38 renovation-specific items ready for
automatic offerte generation from Word document uploads.
</commit_message>
<xml_diff>
--- a/backend/Juiste opnamelijst.xlsx
+++ b/backend/Juiste opnamelijst.xlsx
@@ -1482,7 +1482,7 @@
       </c>
       <c r="B11" s="9" t="inlineStr">
         <is>
-          <t>Toiletrenovatie gemiddeld 1.10 m² incl. fontein</t>
+          <t>Toiletrenovatie gemiddeld 1,10 m² incl. fontein</t>
         </is>
       </c>
       <c r="C11" s="7" t="n">
@@ -1551,7 +1551,7 @@
       </c>
       <c r="Y11" s="7" t="inlineStr">
         <is>
-          <t>Toiletrenovatie gemiddeld 1.10 m² incl. fontein</t>
+          <t>Toiletrenovatie gemiddeld 1,10 m² incl. fontein</t>
         </is>
       </c>
     </row>
@@ -2133,36 +2133,62 @@
           <t>afvalcontainer open 10 m3 alleen van toepassing bij werkzaamheden buiten het prijzenboek om</t>
         </is>
       </c>
-      <c r="C19" s="7" t="n"/>
-      <c r="D19" s="7" t="n"/>
-      <c r="E19" s="7" t="n"/>
-      <c r="F19" s="7" t="n"/>
-      <c r="G19" s="7" t="n"/>
-      <c r="H19" s="7" t="n"/>
-      <c r="I19" s="7" t="n"/>
-      <c r="J19" s="7" t="n"/>
-      <c r="K19" s="7" t="n"/>
-      <c r="L19" s="7" t="n"/>
-      <c r="M19" s="7" t="n"/>
-      <c r="N19" s="7" t="n"/>
-      <c r="O19" s="7" t="n"/>
+      <c r="C19" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L19" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M19" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N19" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O19" s="7" t="n">
+        <v>0</v>
+      </c>
       <c r="P19" s="10" t="n"/>
       <c r="Q19" s="11" t="n">
         <v>0</v>
       </c>
       <c r="R19" s="12" t="inlineStr">
         <is>
-          <t xml:space="preserve">stu       </t>
+          <t>stu</t>
         </is>
       </c>
       <c r="S19" s="13" t="n">
-        <v>434.5000000000001</v>
+        <v>434.5</v>
       </c>
       <c r="T19" s="13" t="n">
         <v>0</v>
       </c>
       <c r="U19" s="13" t="n">
-        <v>434.5000000000001</v>
+        <v>434.5</v>
       </c>
       <c r="V19" s="10" t="n"/>
       <c r="W19" s="14" t="n">
@@ -2188,26 +2214,52 @@
           <t>puincontainer open-schoon puin 6 m3 alleen van toepassing bij werkzaamheden buiten het prijzenboek om</t>
         </is>
       </c>
-      <c r="C20" s="7" t="n"/>
-      <c r="D20" s="7" t="n"/>
-      <c r="E20" s="7" t="n"/>
-      <c r="F20" s="7" t="n"/>
-      <c r="G20" s="7" t="n"/>
-      <c r="H20" s="7" t="n"/>
-      <c r="I20" s="7" t="n"/>
-      <c r="J20" s="7" t="n"/>
-      <c r="K20" s="7" t="n"/>
-      <c r="L20" s="7" t="n"/>
-      <c r="M20" s="7" t="n"/>
-      <c r="N20" s="7" t="n"/>
-      <c r="O20" s="7" t="n"/>
+      <c r="C20" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L20" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M20" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N20" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O20" s="7" t="n">
+        <v>0</v>
+      </c>
       <c r="P20" s="10" t="n"/>
       <c r="Q20" s="11" t="n">
         <v>0</v>
       </c>
       <c r="R20" s="12" t="inlineStr">
         <is>
-          <t xml:space="preserve">stu       </t>
+          <t>stu</t>
         </is>
       </c>
       <c r="S20" s="13" t="n">
@@ -2243,26 +2295,52 @@
           <t>puincontainer open-schoon puin 10 m3 alleen van toepassing bij werkzaamheden buiten het prijzenboek om</t>
         </is>
       </c>
-      <c r="C21" s="7" t="n"/>
-      <c r="D21" s="7" t="n"/>
-      <c r="E21" s="7" t="n"/>
-      <c r="F21" s="7" t="n"/>
-      <c r="G21" s="7" t="n"/>
-      <c r="H21" s="7" t="n"/>
-      <c r="I21" s="7" t="n"/>
-      <c r="J21" s="7" t="n"/>
-      <c r="K21" s="7" t="n"/>
-      <c r="L21" s="7" t="n"/>
-      <c r="M21" s="7" t="n"/>
-      <c r="N21" s="7" t="n"/>
-      <c r="O21" s="7" t="n"/>
+      <c r="C21" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L21" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M21" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N21" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O21" s="7" t="n">
+        <v>0</v>
+      </c>
       <c r="P21" s="10" t="n"/>
       <c r="Q21" s="11" t="n">
         <v>0</v>
       </c>
       <c r="R21" s="12" t="inlineStr">
         <is>
-          <t xml:space="preserve">stu       </t>
+          <t>stu</t>
         </is>
       </c>
       <c r="S21" s="13" t="n">
@@ -2298,36 +2376,62 @@
           <t>afvalcontainer open 15 m3 alleen van toepassing bij werkzaamheden buiten het prijzenboek om</t>
         </is>
       </c>
-      <c r="C22" s="7" t="n"/>
-      <c r="D22" s="7" t="n"/>
-      <c r="E22" s="7" t="n"/>
-      <c r="F22" s="7" t="n"/>
-      <c r="G22" s="7" t="n"/>
-      <c r="H22" s="7" t="n"/>
-      <c r="I22" s="7" t="n"/>
-      <c r="J22" s="7" t="n"/>
-      <c r="K22" s="7" t="n"/>
-      <c r="L22" s="7" t="n"/>
-      <c r="M22" s="7" t="n"/>
-      <c r="N22" s="7" t="n"/>
-      <c r="O22" s="7" t="n"/>
+      <c r="C22" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K22" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L22" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M22" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N22" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O22" s="7" t="n">
+        <v>0</v>
+      </c>
       <c r="P22" s="10" t="n"/>
       <c r="Q22" s="11" t="n">
         <v>0</v>
       </c>
       <c r="R22" s="12" t="inlineStr">
         <is>
-          <t xml:space="preserve">stu       </t>
+          <t>stu</t>
         </is>
       </c>
       <c r="S22" s="13" t="n">
-        <v>836.0000000000001</v>
+        <v>836</v>
       </c>
       <c r="T22" s="13" t="n">
         <v>0</v>
       </c>
       <c r="U22" s="13" t="n">
-        <v>836.0000000000001</v>
+        <v>836</v>
       </c>
       <c r="V22" s="10" t="n"/>
       <c r="W22" s="14" t="n">
@@ -2353,26 +2457,52 @@
           <t>puincontainer open-schoon puin 15 m3 alleen van toepassing bij werkzaamheden buiten het prijzenboek om</t>
         </is>
       </c>
-      <c r="C23" s="7" t="n"/>
-      <c r="D23" s="7" t="n"/>
-      <c r="E23" s="7" t="n"/>
-      <c r="F23" s="7" t="n"/>
-      <c r="G23" s="7" t="n"/>
-      <c r="H23" s="7" t="n"/>
-      <c r="I23" s="7" t="n"/>
-      <c r="J23" s="7" t="n"/>
-      <c r="K23" s="7" t="n"/>
-      <c r="L23" s="7" t="n"/>
-      <c r="M23" s="7" t="n"/>
-      <c r="N23" s="7" t="n"/>
-      <c r="O23" s="7" t="n"/>
+      <c r="C23" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I23" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K23" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L23" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M23" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N23" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O23" s="7" t="n">
+        <v>0</v>
+      </c>
       <c r="P23" s="10" t="n"/>
       <c r="Q23" s="11" t="n">
         <v>0</v>
       </c>
       <c r="R23" s="12" t="inlineStr">
         <is>
-          <t xml:space="preserve">stu       </t>
+          <t>stu</t>
         </is>
       </c>
       <c r="S23" s="13" t="n">
@@ -2408,26 +2538,52 @@
           <t>puincontainer gesloten 10 m3 schoon puin alleen van toepassing bij werkzaamheden buiten het prijzenboek om</t>
         </is>
       </c>
-      <c r="C24" s="7" t="n"/>
-      <c r="D24" s="7" t="n"/>
-      <c r="E24" s="7" t="n"/>
-      <c r="F24" s="7" t="n"/>
-      <c r="G24" s="7" t="n"/>
-      <c r="H24" s="7" t="n"/>
-      <c r="I24" s="7" t="n"/>
-      <c r="J24" s="7" t="n"/>
-      <c r="K24" s="7" t="n"/>
-      <c r="L24" s="7" t="n"/>
-      <c r="M24" s="7" t="n"/>
-      <c r="N24" s="7" t="n"/>
-      <c r="O24" s="7" t="n"/>
+      <c r="C24" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K24" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L24" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M24" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N24" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O24" s="7" t="n">
+        <v>0</v>
+      </c>
       <c r="P24" s="10" t="n"/>
       <c r="Q24" s="11" t="n">
         <v>0</v>
       </c>
       <c r="R24" s="12" t="inlineStr">
         <is>
-          <t xml:space="preserve">stu       </t>
+          <t>stu</t>
         </is>
       </c>
       <c r="S24" s="13" t="n">
@@ -2463,26 +2619,52 @@
           <t>afvalcontainer open 3 m3 alleen van toepassing bij werkzaamheden buiten het prijzenboek om</t>
         </is>
       </c>
-      <c r="C25" s="7" t="n"/>
-      <c r="D25" s="7" t="n"/>
-      <c r="E25" s="7" t="n"/>
-      <c r="F25" s="7" t="n"/>
-      <c r="G25" s="7" t="n"/>
-      <c r="H25" s="7" t="n"/>
-      <c r="I25" s="7" t="n"/>
-      <c r="J25" s="7" t="n"/>
-      <c r="K25" s="7" t="n"/>
-      <c r="L25" s="7" t="n"/>
-      <c r="M25" s="7" t="n"/>
-      <c r="N25" s="7" t="n"/>
-      <c r="O25" s="7" t="n"/>
+      <c r="C25" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J25" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K25" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L25" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M25" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N25" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O25" s="7" t="n">
+        <v>0</v>
+      </c>
       <c r="P25" s="10" t="n"/>
       <c r="Q25" s="11" t="n">
         <v>0</v>
       </c>
       <c r="R25" s="12" t="inlineStr">
         <is>
-          <t xml:space="preserve">stu       </t>
+          <t>stu</t>
         </is>
       </c>
       <c r="S25" s="13" t="n">
@@ -2518,26 +2700,52 @@
           <t>puincontainer open-schoon puin 3 m3 alleen van toepassing bij werkzaamheden buiten het prijzenboek om</t>
         </is>
       </c>
-      <c r="C26" s="7" t="n"/>
-      <c r="D26" s="7" t="n"/>
-      <c r="E26" s="7" t="n"/>
-      <c r="F26" s="7" t="n"/>
-      <c r="G26" s="7" t="n"/>
-      <c r="H26" s="7" t="n"/>
-      <c r="I26" s="7" t="n"/>
-      <c r="J26" s="7" t="n"/>
-      <c r="K26" s="7" t="n"/>
-      <c r="L26" s="7" t="n"/>
-      <c r="M26" s="7" t="n"/>
-      <c r="N26" s="7" t="n"/>
-      <c r="O26" s="7" t="n"/>
+      <c r="C26" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K26" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L26" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M26" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N26" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O26" s="7" t="n">
+        <v>0</v>
+      </c>
       <c r="P26" s="10" t="n"/>
       <c r="Q26" s="11" t="n">
         <v>0</v>
       </c>
       <c r="R26" s="12" t="inlineStr">
         <is>
-          <t xml:space="preserve">stu       </t>
+          <t>stu</t>
         </is>
       </c>
       <c r="S26" s="13" t="n">
@@ -2573,26 +2781,52 @@
           <t>woning bezemschoon opleveren</t>
         </is>
       </c>
-      <c r="C27" s="7" t="n"/>
-      <c r="D27" s="7" t="n"/>
-      <c r="E27" s="7" t="n"/>
-      <c r="F27" s="7" t="n"/>
-      <c r="G27" s="7" t="n"/>
-      <c r="H27" s="7" t="n"/>
-      <c r="I27" s="7" t="n"/>
-      <c r="J27" s="7" t="n"/>
-      <c r="K27" s="7" t="n"/>
-      <c r="L27" s="7" t="n"/>
-      <c r="M27" s="7" t="n"/>
-      <c r="N27" s="7" t="n"/>
-      <c r="O27" s="7" t="n"/>
+      <c r="C27" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K27" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L27" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M27" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N27" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O27" s="7" t="n">
+        <v>0</v>
+      </c>
       <c r="P27" s="10" t="n"/>
       <c r="Q27" s="11" t="n">
         <v>0</v>
       </c>
       <c r="R27" s="12" t="inlineStr">
         <is>
-          <t xml:space="preserve">won       </t>
+          <t>won</t>
         </is>
       </c>
       <c r="S27" s="13" t="n">
@@ -2628,36 +2862,62 @@
           <t>woning nat reinigen/schoonmaken</t>
         </is>
       </c>
-      <c r="C28" s="7" t="n"/>
-      <c r="D28" s="7" t="n"/>
-      <c r="E28" s="7" t="n"/>
-      <c r="F28" s="7" t="n"/>
-      <c r="G28" s="7" t="n"/>
-      <c r="H28" s="7" t="n"/>
-      <c r="I28" s="7" t="n"/>
-      <c r="J28" s="7" t="n"/>
-      <c r="K28" s="7" t="n"/>
-      <c r="L28" s="7" t="n"/>
-      <c r="M28" s="7" t="n"/>
-      <c r="N28" s="7" t="n"/>
-      <c r="O28" s="7" t="n"/>
+      <c r="C28" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K28" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L28" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M28" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N28" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O28" s="7" t="n">
+        <v>0</v>
+      </c>
       <c r="P28" s="10" t="n"/>
       <c r="Q28" s="11" t="n">
         <v>0</v>
       </c>
       <c r="R28" s="12" t="inlineStr">
         <is>
-          <t xml:space="preserve">won       </t>
+          <t>won</t>
         </is>
       </c>
       <c r="S28" s="13" t="n">
-        <v>3.366000000000001</v>
+        <v>3.37</v>
       </c>
       <c r="T28" s="13" t="n">
-        <v>214.5975</v>
+        <v>214.6</v>
       </c>
       <c r="U28" s="13" t="n">
-        <v>217.9635</v>
+        <v>217.96</v>
       </c>
       <c r="V28" s="10" t="n"/>
       <c r="W28" s="14" t="n">
@@ -2683,36 +2943,62 @@
           <t>keukenruimte incl keukenblok, aanrechtblad en bovenkasten reinigen/schoonmaken</t>
         </is>
       </c>
-      <c r="C29" s="7" t="n"/>
-      <c r="D29" s="7" t="n"/>
-      <c r="E29" s="7" t="n"/>
-      <c r="F29" s="7" t="n"/>
-      <c r="G29" s="7" t="n"/>
-      <c r="H29" s="7" t="n"/>
-      <c r="I29" s="7" t="n"/>
-      <c r="J29" s="7" t="n"/>
-      <c r="K29" s="7" t="n"/>
-      <c r="L29" s="7" t="n"/>
-      <c r="M29" s="7" t="n"/>
-      <c r="N29" s="7" t="n"/>
-      <c r="O29" s="7" t="n"/>
+      <c r="C29" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I29" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J29" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K29" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L29" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M29" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N29" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O29" s="7" t="n">
+        <v>0</v>
+      </c>
       <c r="P29" s="10" t="n"/>
       <c r="Q29" s="11" t="n">
         <v>0</v>
       </c>
       <c r="R29" s="12" t="inlineStr">
         <is>
-          <t xml:space="preserve">stu       </t>
+          <t>stu</t>
         </is>
       </c>
       <c r="S29" s="13" t="n">
-        <v>3.366000000000001</v>
+        <v>3.37</v>
       </c>
       <c r="T29" s="13" t="n">
-        <v>49.5225</v>
+        <v>49.52</v>
       </c>
       <c r="U29" s="13" t="n">
-        <v>52.8885</v>
+        <v>52.89</v>
       </c>
       <c r="V29" s="10" t="n"/>
       <c r="W29" s="14" t="n">
@@ -2738,36 +3024,62 @@
           <t>woning per ruimte beschermen/afdekken</t>
         </is>
       </c>
-      <c r="C30" s="7" t="n"/>
-      <c r="D30" s="7" t="n"/>
-      <c r="E30" s="7" t="n"/>
-      <c r="F30" s="7" t="n"/>
-      <c r="G30" s="7" t="n"/>
-      <c r="H30" s="7" t="n"/>
-      <c r="I30" s="7" t="n"/>
-      <c r="J30" s="7" t="n"/>
-      <c r="K30" s="7" t="n"/>
-      <c r="L30" s="7" t="n"/>
-      <c r="M30" s="7" t="n"/>
-      <c r="N30" s="7" t="n"/>
-      <c r="O30" s="7" t="n"/>
+      <c r="C30" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I30" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K30" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L30" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M30" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N30" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O30" s="7" t="n">
+        <v>0</v>
+      </c>
       <c r="P30" s="10" t="n"/>
       <c r="Q30" s="11" t="n">
         <v>0</v>
       </c>
       <c r="R30" s="12" t="inlineStr">
         <is>
-          <t xml:space="preserve">ruimte    </t>
+          <t>ruimte</t>
         </is>
       </c>
       <c r="S30" s="13" t="n">
         <v>11.22</v>
       </c>
       <c r="T30" s="13" t="n">
-        <v>26.412</v>
+        <v>26.41</v>
       </c>
       <c r="U30" s="13" t="n">
-        <v>37.63200000000001</v>
+        <v>37.63</v>
       </c>
       <c r="V30" s="10" t="n"/>
       <c r="W30" s="14" t="n">
@@ -2793,36 +3105,62 @@
           <t>woning per m2 beschermen/afdekken</t>
         </is>
       </c>
-      <c r="C31" s="7" t="n"/>
-      <c r="D31" s="7" t="n"/>
-      <c r="E31" s="7" t="n"/>
-      <c r="F31" s="7" t="n"/>
-      <c r="G31" s="7" t="n"/>
-      <c r="H31" s="7" t="n"/>
-      <c r="I31" s="7" t="n"/>
-      <c r="J31" s="7" t="n"/>
-      <c r="K31" s="7" t="n"/>
-      <c r="L31" s="7" t="n"/>
-      <c r="M31" s="7" t="n"/>
-      <c r="N31" s="7" t="n"/>
-      <c r="O31" s="7" t="n"/>
+      <c r="C31" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I31" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J31" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K31" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L31" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M31" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N31" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O31" s="7" t="n">
+        <v>0</v>
+      </c>
       <c r="P31" s="10" t="n"/>
       <c r="Q31" s="11" t="n">
         <v>0</v>
       </c>
       <c r="R31" s="12" t="inlineStr">
         <is>
-          <t xml:space="preserve">m2        </t>
+          <t>m2</t>
         </is>
       </c>
       <c r="S31" s="13" t="n">
-        <v>1.122</v>
+        <v>1.12</v>
       </c>
       <c r="T31" s="13" t="n">
-        <v>2.6412</v>
+        <v>2.64</v>
       </c>
       <c r="U31" s="13" t="n">
-        <v>3.7632</v>
+        <v>3.76</v>
       </c>
       <c r="V31" s="10" t="n"/>
       <c r="W31" s="14" t="n">
@@ -2848,36 +3186,62 @@
           <t>vervuilde woning nat reinigen/schoonmaken</t>
         </is>
       </c>
-      <c r="C32" s="7" t="n"/>
-      <c r="D32" s="7" t="n"/>
-      <c r="E32" s="7" t="n"/>
-      <c r="F32" s="7" t="n"/>
-      <c r="G32" s="7" t="n"/>
-      <c r="H32" s="7" t="n"/>
-      <c r="I32" s="7" t="n"/>
-      <c r="J32" s="7" t="n"/>
-      <c r="K32" s="7" t="n"/>
-      <c r="L32" s="7" t="n"/>
-      <c r="M32" s="7" t="n"/>
-      <c r="N32" s="7" t="n"/>
-      <c r="O32" s="7" t="n"/>
+      <c r="C32" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I32" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J32" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K32" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L32" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M32" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N32" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O32" s="7" t="n">
+        <v>0</v>
+      </c>
       <c r="P32" s="10" t="n"/>
       <c r="Q32" s="11" t="n">
         <v>0</v>
       </c>
       <c r="R32" s="12" t="inlineStr">
         <is>
-          <t xml:space="preserve">won       </t>
+          <t>won</t>
         </is>
       </c>
       <c r="S32" s="13" t="n">
-        <v>3.366000000000001</v>
+        <v>3.37</v>
       </c>
       <c r="T32" s="13" t="n">
-        <v>297.135</v>
+        <v>297.14</v>
       </c>
       <c r="U32" s="13" t="n">
-        <v>300.501</v>
+        <v>300.5</v>
       </c>
       <c r="V32" s="10" t="n"/>
       <c r="W32" s="14" t="n">
@@ -2903,36 +3267,62 @@
           <t>keukenblok, aanrechtblad en bovenkasten (bij sterke vervuiling) reinigen/schoonmaken</t>
         </is>
       </c>
-      <c r="C33" s="7" t="n"/>
-      <c r="D33" s="7" t="n"/>
-      <c r="E33" s="7" t="n"/>
-      <c r="F33" s="7" t="n"/>
-      <c r="G33" s="7" t="n"/>
-      <c r="H33" s="7" t="n"/>
-      <c r="I33" s="7" t="n"/>
-      <c r="J33" s="7" t="n"/>
-      <c r="K33" s="7" t="n"/>
-      <c r="L33" s="7" t="n"/>
-      <c r="M33" s="7" t="n"/>
-      <c r="N33" s="7" t="n"/>
-      <c r="O33" s="7" t="n"/>
+      <c r="C33" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I33" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J33" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K33" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L33" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M33" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N33" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O33" s="7" t="n">
+        <v>0</v>
+      </c>
       <c r="P33" s="10" t="n"/>
       <c r="Q33" s="11" t="n">
         <v>0</v>
       </c>
       <c r="R33" s="12" t="inlineStr">
         <is>
-          <t xml:space="preserve">stu       </t>
+          <t>stu</t>
         </is>
       </c>
       <c r="S33" s="13" t="n">
-        <v>3.366000000000001</v>
+        <v>3.37</v>
       </c>
       <c r="T33" s="13" t="n">
-        <v>99.045</v>
+        <v>99.05</v>
       </c>
       <c r="U33" s="13" t="n">
-        <v>102.411</v>
+        <v>102.41</v>
       </c>
       <c r="V33" s="10" t="n"/>
       <c r="W33" s="14" t="n">
@@ -2958,36 +3348,62 @@
           <t>woning nat reinigen/schoonmaken per bvo</t>
         </is>
       </c>
-      <c r="C34" s="7" t="n"/>
-      <c r="D34" s="7" t="n"/>
-      <c r="E34" s="7" t="n"/>
-      <c r="F34" s="7" t="n"/>
-      <c r="G34" s="7" t="n"/>
-      <c r="H34" s="7" t="n"/>
-      <c r="I34" s="7" t="n"/>
-      <c r="J34" s="7" t="n"/>
-      <c r="K34" s="7" t="n"/>
-      <c r="L34" s="7" t="n"/>
-      <c r="M34" s="7" t="n"/>
-      <c r="N34" s="7" t="n"/>
-      <c r="O34" s="7" t="n"/>
+      <c r="C34" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G34" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I34" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J34" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K34" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L34" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M34" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N34" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O34" s="7" t="n">
+        <v>0</v>
+      </c>
       <c r="P34" s="10" t="n"/>
       <c r="Q34" s="11" t="n">
         <v>0</v>
       </c>
       <c r="R34" s="12" t="inlineStr">
         <is>
-          <t xml:space="preserve">m2        </t>
+          <t>m2</t>
         </is>
       </c>
       <c r="S34" s="13" t="n">
-        <v>0.044</v>
+        <v>0.04</v>
       </c>
       <c r="T34" s="13" t="n">
-        <v>2.717101485</v>
+        <v>2.72</v>
       </c>
       <c r="U34" s="13" t="n">
-        <v>2.761101485</v>
+        <v>2.76</v>
       </c>
       <c r="V34" s="10" t="n"/>
       <c r="W34" s="14" t="n">
@@ -3013,36 +3429,62 @@
           <t>radiator reinigen/schoonmaken (niet combineren met schilderwerk)</t>
         </is>
       </c>
-      <c r="C35" s="7" t="n"/>
-      <c r="D35" s="7" t="n"/>
-      <c r="E35" s="7" t="n"/>
-      <c r="F35" s="7" t="n"/>
-      <c r="G35" s="7" t="n"/>
-      <c r="H35" s="7" t="n"/>
-      <c r="I35" s="7" t="n"/>
-      <c r="J35" s="7" t="n"/>
-      <c r="K35" s="7" t="n"/>
-      <c r="L35" s="7" t="n"/>
-      <c r="M35" s="7" t="n"/>
-      <c r="N35" s="7" t="n"/>
-      <c r="O35" s="7" t="n"/>
+      <c r="C35" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I35" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J35" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K35" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L35" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M35" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N35" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O35" s="7" t="n">
+        <v>0</v>
+      </c>
       <c r="P35" s="10" t="n"/>
       <c r="Q35" s="11" t="n">
         <v>0</v>
       </c>
       <c r="R35" s="12" t="inlineStr">
         <is>
-          <t xml:space="preserve">stu       </t>
+          <t>stu</t>
         </is>
       </c>
       <c r="S35" s="13" t="n">
-        <v>2.662</v>
+        <v>2.66</v>
       </c>
       <c r="T35" s="13" t="n">
-        <v>16.5075</v>
+        <v>16.51</v>
       </c>
       <c r="U35" s="13" t="n">
-        <v>19.1695</v>
+        <v>19.17</v>
       </c>
       <c r="V35" s="10" t="n"/>
       <c r="W35" s="14" t="n">
@@ -3068,36 +3510,62 @@
           <t>sanitair reinigen/schoonmaken incl. kalkaanslag verwijderen (niet combineren met renovaties)</t>
         </is>
       </c>
-      <c r="C36" s="7" t="n"/>
-      <c r="D36" s="7" t="n"/>
-      <c r="E36" s="7" t="n"/>
-      <c r="F36" s="7" t="n"/>
-      <c r="G36" s="7" t="n"/>
-      <c r="H36" s="7" t="n"/>
-      <c r="I36" s="7" t="n"/>
-      <c r="J36" s="7" t="n"/>
-      <c r="K36" s="7" t="n"/>
-      <c r="L36" s="7" t="n"/>
-      <c r="M36" s="7" t="n"/>
-      <c r="N36" s="7" t="n"/>
-      <c r="O36" s="7" t="n"/>
+      <c r="C36" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H36" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I36" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J36" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K36" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L36" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M36" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N36" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O36" s="7" t="n">
+        <v>0</v>
+      </c>
       <c r="P36" s="10" t="n"/>
       <c r="Q36" s="11" t="n">
         <v>0</v>
       </c>
       <c r="R36" s="12" t="inlineStr">
         <is>
-          <t xml:space="preserve">stu       </t>
+          <t>stu</t>
         </is>
       </c>
       <c r="S36" s="13" t="n">
-        <v>2.024</v>
+        <v>2.02</v>
       </c>
       <c r="T36" s="13" t="n">
-        <v>23.1105</v>
+        <v>23.11</v>
       </c>
       <c r="U36" s="13" t="n">
-        <v>25.1345</v>
+        <v>25.13</v>
       </c>
       <c r="V36" s="10" t="n"/>
       <c r="W36" s="14" t="n">
@@ -3123,36 +3591,62 @@
           <t>alle plastic folie verwijderen van beglazing in gehele woning</t>
         </is>
       </c>
-      <c r="C37" s="7" t="n"/>
-      <c r="D37" s="7" t="n"/>
-      <c r="E37" s="7" t="n"/>
-      <c r="F37" s="7" t="n"/>
-      <c r="G37" s="7" t="n"/>
-      <c r="H37" s="7" t="n"/>
-      <c r="I37" s="7" t="n"/>
-      <c r="J37" s="7" t="n"/>
-      <c r="K37" s="7" t="n"/>
-      <c r="L37" s="7" t="n"/>
-      <c r="M37" s="7" t="n"/>
-      <c r="N37" s="7" t="n"/>
-      <c r="O37" s="7" t="n"/>
+      <c r="C37" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G37" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H37" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I37" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J37" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K37" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L37" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M37" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N37" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O37" s="7" t="n">
+        <v>0</v>
+      </c>
       <c r="P37" s="10" t="n"/>
       <c r="Q37" s="11" t="n">
         <v>0</v>
       </c>
       <c r="R37" s="12" t="inlineStr">
         <is>
-          <t xml:space="preserve">won       </t>
+          <t>won</t>
         </is>
       </c>
       <c r="S37" s="13" t="n">
-        <v>0.7260000000000001</v>
+        <v>0.73</v>
       </c>
       <c r="T37" s="13" t="n">
         <v>66.03</v>
       </c>
       <c r="U37" s="13" t="n">
-        <v>66.756</v>
+        <v>66.76000000000001</v>
       </c>
       <c r="V37" s="10" t="n"/>
       <c r="W37" s="14" t="n">
@@ -3178,36 +3672,62 @@
           <t>kraan reinigen/ontkalken  (niet combineren met renovaties)</t>
         </is>
       </c>
-      <c r="C38" s="7" t="n"/>
-      <c r="D38" s="7" t="n"/>
-      <c r="E38" s="7" t="n"/>
-      <c r="F38" s="7" t="n"/>
-      <c r="G38" s="7" t="n"/>
-      <c r="H38" s="7" t="n"/>
-      <c r="I38" s="7" t="n"/>
-      <c r="J38" s="7" t="n"/>
-      <c r="K38" s="7" t="n"/>
-      <c r="L38" s="7" t="n"/>
-      <c r="M38" s="7" t="n"/>
-      <c r="N38" s="7" t="n"/>
-      <c r="O38" s="7" t="n"/>
+      <c r="C38" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D38" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F38" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G38" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H38" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I38" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J38" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K38" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L38" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M38" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N38" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O38" s="7" t="n">
+        <v>0</v>
+      </c>
       <c r="P38" s="10" t="n"/>
       <c r="Q38" s="11" t="n">
         <v>0</v>
       </c>
       <c r="R38" s="12" t="inlineStr">
         <is>
-          <t xml:space="preserve">stu       </t>
+          <t>stu</t>
         </is>
       </c>
       <c r="S38" s="13" t="n">
-        <v>1.562</v>
+        <v>1.56</v>
       </c>
       <c r="T38" s="13" t="n">
-        <v>6.603000000000001</v>
+        <v>6.6</v>
       </c>
       <c r="U38" s="13" t="n">
-        <v>8.165000000000001</v>
+        <v>8.17</v>
       </c>
       <c r="V38" s="10" t="n"/>
       <c r="W38" s="14" t="n">
@@ -3233,36 +3753,62 @@
           <t>closetruimte reinigen/schoonmaken incl kalkaanslag verwijderen  (niet combineren met renovaties)</t>
         </is>
       </c>
-      <c r="C39" s="7" t="n"/>
-      <c r="D39" s="7" t="n"/>
-      <c r="E39" s="7" t="n"/>
-      <c r="F39" s="7" t="n"/>
-      <c r="G39" s="7" t="n"/>
-      <c r="H39" s="7" t="n"/>
-      <c r="I39" s="7" t="n"/>
-      <c r="J39" s="7" t="n"/>
-      <c r="K39" s="7" t="n"/>
-      <c r="L39" s="7" t="n"/>
-      <c r="M39" s="7" t="n"/>
-      <c r="N39" s="7" t="n"/>
-      <c r="O39" s="7" t="n"/>
+      <c r="C39" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G39" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H39" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I39" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J39" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K39" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L39" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M39" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N39" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O39" s="7" t="n">
+        <v>0</v>
+      </c>
       <c r="P39" s="10" t="n"/>
       <c r="Q39" s="11" t="n">
         <v>0</v>
       </c>
       <c r="R39" s="12" t="inlineStr">
         <is>
-          <t xml:space="preserve">stu       </t>
+          <t>stu</t>
         </is>
       </c>
       <c r="S39" s="13" t="n">
-        <v>1.298</v>
+        <v>1.3</v>
       </c>
       <c r="T39" s="13" t="n">
-        <v>33.015</v>
+        <v>33.02</v>
       </c>
       <c r="U39" s="13" t="n">
-        <v>34.313</v>
+        <v>34.31</v>
       </c>
       <c r="V39" s="10" t="n"/>
       <c r="W39" s="14" t="n">

</xml_diff>